<commit_message>
not sure whether this commit is correct either
</commit_message>
<xml_diff>
--- a/examples/EU_without_aggregation/InputData/SpatialData/ElectricGrid/cableCapacity_GW_aggregated.xlsx
+++ b/examples/EU_without_aggregation/InputData/SpatialData/ElectricGrid/cableCapacity_GW_aggregated.xlsx
@@ -576,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>81.2</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>217.8</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>39.6</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>24.8</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>262.5499999999999</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>23.2</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -1753,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -1860,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>15.2</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
         <v>0</v>
@@ -2074,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>84.2</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="n">
         <v>1.7</v>
@@ -2181,7 +2181,7 @@
         <v>1.7</v>
       </c>
       <c r="Q17" t="n">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="R17" t="n">
         <v>0</v>
@@ -2288,7 +2288,7 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -2502,7 +2502,7 @@
         <v>1.7</v>
       </c>
       <c r="T20" t="n">
-        <v>22.2</v>
+        <v>0</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -3037,7 +3037,7 @@
         <v>0</v>
       </c>
       <c r="Y25" t="n">
-        <v>228.3</v>
+        <v>0</v>
       </c>
       <c r="Z25" t="n">
         <v>0</v>
@@ -3144,7 +3144,7 @@
         <v>0</v>
       </c>
       <c r="Z26" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AA26" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
fixed and improved data preprocessing
</commit_message>
<xml_diff>
--- a/examples/EU_without_aggregation/InputData/SpatialData/ElectricGrid/cableCapacity_GW_aggregated.xlsx
+++ b/examples/EU_without_aggregation/InputData/SpatialData/ElectricGrid/cableCapacity_GW_aggregated.xlsx
@@ -12,110 +12,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
-  <si>
-    <t>pl</t>
-  </si>
-  <si>
-    <t>es</t>
-  </si>
-  <si>
-    <t>ch</t>
-  </si>
-  <si>
-    <t>se</t>
-  </si>
-  <si>
-    <t>sk</t>
-  </si>
-  <si>
-    <t>lu</t>
-  </si>
-  <si>
-    <t>at</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>ba</t>
-  </si>
-  <si>
-    <t>gr</t>
-  </si>
-  <si>
-    <t>uk</t>
-  </si>
-  <si>
-    <t>pt</t>
-  </si>
-  <si>
-    <t>cz</t>
-  </si>
-  <si>
-    <t>be</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>dk</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>bg</t>
-  </si>
-  <si>
-    <t>ro</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>hu</t>
-  </si>
-  <si>
-    <t>mk</t>
-  </si>
-  <si>
-    <t>hr</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>fi</t>
-  </si>
-  <si>
-    <t>nl</t>
-  </si>
-  <si>
-    <t>ie</t>
-  </si>
-  <si>
-    <t>lv</t>
-  </si>
-  <si>
-    <t>al</t>
-  </si>
-  <si>
-    <t>si</t>
-  </si>
-  <si>
-    <t>rs</t>
-  </si>
-  <si>
-    <t>lt</t>
-  </si>
-  <si>
-    <t>me</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,110 +366,178 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>32</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pl</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ch</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>se</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>sk</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>lu</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>at</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ba</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>gr</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>uk</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>cz</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>be</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>dk</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>bg</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>ro</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>ee</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>hu</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>mk</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>hr</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>fi</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>nl</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>ie</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>lv</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>al</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>rs</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>lt</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:34">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>pl</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -675,9 +639,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -779,9 +745,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>ch</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -883,9 +851,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>se</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>0.6</v>
@@ -987,9 +957,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>sk</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>0.6</v>
@@ -1091,9 +1063,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>lu</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1195,9 +1169,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>at</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -1299,9 +1275,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -1403,9 +1381,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>ba</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -1507,9 +1487,11 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>gr</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -1611,9 +1593,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>uk</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -1715,9 +1699,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>pt</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -1819,9 +1805,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>cz</t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>4.1</v>
@@ -1923,9 +1911,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>be</t>
+        </is>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -2027,9 +2017,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -2131,9 +2123,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:34">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>dk</t>
+        </is>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -2235,9 +2229,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:34">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -2339,9 +2335,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:34">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>bg</t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -2443,9 +2441,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:34">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>ro</t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -2547,9 +2547,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:34">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>ee</t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -2651,9 +2653,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:34">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>hu</t>
+        </is>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -2755,9 +2759,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:34">
-      <c r="A23" s="1" t="s">
-        <v>21</v>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>mk</t>
+        </is>
       </c>
       <c r="B23" t="n">
         <v>0</v>
@@ -2859,9 +2865,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:34">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>hr</t>
+        </is>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -2963,9 +2971,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:34">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>de</t>
+        </is>
       </c>
       <c r="B25" t="n">
         <v>15.1</v>
@@ -3067,9 +3077,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:34">
-      <c r="A26" s="1" t="s">
-        <v>24</v>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>fi</t>
+        </is>
       </c>
       <c r="B26" t="n">
         <v>0</v>
@@ -3171,9 +3183,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:34">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>nl</t>
+        </is>
       </c>
       <c r="B27" t="n">
         <v>0</v>
@@ -3275,9 +3289,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:34">
-      <c r="A28" s="1" t="s">
-        <v>26</v>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>ie</t>
+        </is>
       </c>
       <c r="B28" t="n">
         <v>0</v>
@@ -3379,9 +3395,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:34">
-      <c r="A29" s="1" t="s">
-        <v>27</v>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>lv</t>
+        </is>
       </c>
       <c r="B29" t="n">
         <v>0</v>
@@ -3483,9 +3501,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:34">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>al</t>
+        </is>
       </c>
       <c r="B30" t="n">
         <v>0</v>
@@ -3587,9 +3607,11 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="31" spans="1:34">
-      <c r="A31" s="1" t="s">
-        <v>29</v>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
       </c>
       <c r="B31" t="n">
         <v>0</v>
@@ -3691,9 +3713,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:34">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>rs</t>
+        </is>
       </c>
       <c r="B32" t="n">
         <v>0</v>
@@ -3795,9 +3819,11 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="33" spans="1:34">
-      <c r="A33" s="1" t="s">
-        <v>31</v>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>lt</t>
+        </is>
       </c>
       <c r="B33" t="n">
         <v>9</v>
@@ -3899,9 +3925,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:34">
-      <c r="A34" s="1" t="s">
-        <v>32</v>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
       </c>
       <c r="B34" t="n">
         <v>0</v>

</xml_diff>